<commit_message>
Parameter tuning for GA configuration
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -577,10 +577,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G2" t="n">
         <v>40</v>
@@ -690,7 +690,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3" t="n">
         <v>40</v>
@@ -797,10 +797,10 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G4" t="n">
         <v>40</v>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>10</v>
@@ -1020,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>40</v>
@@ -1127,10 +1127,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G7" t="n">
         <v>80</v>
@@ -1237,10 +1237,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
         <v>80</v>
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>3</v>
@@ -1460,7 +1460,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G10" t="n">
         <v>80</v>
@@ -1567,16 +1567,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G11" t="n">
         <v>40</v>
       </c>
       <c r="H11" t="n">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1677,10 +1677,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
         <v>40</v>
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G13" t="n">
         <v>40</v>
@@ -1897,10 +1897,10 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G14" t="n">
         <v>40</v>
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>9</v>
@@ -2117,10 +2117,10 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G16" t="n">
         <v>160</v>
@@ -2227,16 +2227,16 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
         <v>160</v>
       </c>
       <c r="H17" t="n">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -2337,10 +2337,10 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G18" t="n">
         <v>160</v>
@@ -2447,10 +2447,10 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G19" t="n">
         <v>160</v>
@@ -2557,10 +2557,10 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" t="n">
         <v>160</v>
@@ -2667,16 +2667,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G21" t="n">
         <v>160</v>
       </c>
       <c r="H21" t="n">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -2777,10 +2777,10 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" t="n">
         <v>160</v>
@@ -2997,16 +2997,16 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F24" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G24" t="n">
         <v>160</v>
       </c>
       <c r="H24" t="n">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -3107,10 +3107,10 @@
         </is>
       </c>
       <c r="E25" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" t="n">
         <v>7</v>
-      </c>
-      <c r="F25" t="n">
-        <v>8</v>
       </c>
       <c r="G25" t="n">
         <v>160</v>
@@ -3217,10 +3217,10 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G26" t="n">
         <v>160</v>
@@ -3330,7 +3330,7 @@
         <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G27" t="n">
         <v>160</v>
@@ -3437,10 +3437,10 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G28" t="n">
         <v>160</v>
@@ -3547,7 +3547,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
         <v>8</v>
@@ -3657,10 +3657,10 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G30" t="n">
         <v>160</v>
@@ -3877,10 +3877,10 @@
         </is>
       </c>
       <c r="E32" t="n">
+        <v>7</v>
+      </c>
+      <c r="F32" t="n">
         <v>3</v>
-      </c>
-      <c r="F32" t="n">
-        <v>9</v>
       </c>
       <c r="G32" t="n">
         <v>160</v>
@@ -3987,10 +3987,10 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G33" t="n">
         <v>160</v>
@@ -4100,7 +4100,7 @@
         <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G34" t="n">
         <v>160</v>
@@ -4207,10 +4207,10 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G35" t="n">
         <v>160</v>
@@ -4317,10 +4317,10 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F36" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
         <v>160</v>
@@ -4427,10 +4427,10 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G37" t="n">
         <v>160</v>
@@ -4537,10 +4537,10 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G38" t="n">
         <v>140</v>
@@ -4647,10 +4647,10 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G39" t="n">
         <v>140</v>
@@ -4757,10 +4757,10 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G40" t="n">
         <v>140</v>
@@ -4867,10 +4867,10 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G41" t="n">
         <v>140</v>
@@ -4977,16 +4977,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G42" t="n">
         <v>140</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -5087,10 +5087,10 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G43" t="n">
         <v>140</v>
@@ -5200,7 +5200,7 @@
         <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G44" t="n">
         <v>140</v>
@@ -5417,10 +5417,10 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G46" t="n">
         <v>140</v>
@@ -5527,7 +5527,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F47" t="n">
         <v>11</v>
@@ -5637,16 +5637,16 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F48" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G48" t="n">
         <v>140</v>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -5747,10 +5747,10 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G49" t="n">
         <v>140</v>
@@ -5857,10 +5857,10 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G50" t="n">
         <v>140</v>
@@ -5967,10 +5967,10 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G51" t="n">
         <v>140</v>
@@ -6077,10 +6077,10 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F52" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G52" t="n">
         <v>80</v>
@@ -6187,10 +6187,10 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F53" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G53" t="n">
         <v>80</v>
@@ -6297,10 +6297,10 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G54" t="n">
         <v>80</v>
@@ -6407,10 +6407,10 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G55" t="n">
         <v>80</v>
@@ -6517,10 +6517,10 @@
         </is>
       </c>
       <c r="E56" t="n">
+        <v>3</v>
+      </c>
+      <c r="F56" t="n">
         <v>5</v>
-      </c>
-      <c r="F56" t="n">
-        <v>7</v>
       </c>
       <c r="G56" t="n">
         <v>80</v>
@@ -6627,7 +6627,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>2</v>
@@ -6737,10 +6737,10 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G58" t="n">
         <v>80</v>
@@ -6847,10 +6847,10 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G59" t="n">
         <v>80</v>
@@ -6957,10 +6957,10 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G60" t="n">
         <v>80</v>
@@ -7067,10 +7067,10 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G61" t="n">
         <v>80</v>
@@ -7177,7 +7177,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F62" t="n">
         <v>7</v>
@@ -7290,7 +7290,7 @@
         <v>3</v>
       </c>
       <c r="F63" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G63" t="n">
         <v>60</v>
@@ -7397,10 +7397,10 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F64" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G64" t="n">
         <v>60</v>
@@ -7617,7 +7617,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="n">
         <v>10</v>
@@ -7730,7 +7730,7 @@
         <v>2</v>
       </c>
       <c r="F67" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G67" t="n">
         <v>80</v>
@@ -7837,10 +7837,10 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F68" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G68" t="n">
         <v>80</v>
@@ -7947,16 +7947,16 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G69" t="n">
         <v>80</v>
       </c>
       <c r="H69" t="n">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
@@ -8057,10 +8057,10 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G70" t="n">
         <v>80</v>
@@ -8170,7 +8170,7 @@
         <v>3</v>
       </c>
       <c r="F71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G71" t="n">
         <v>80</v>
@@ -8277,10 +8277,10 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F72" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G72" t="n">
         <v>80</v>
@@ -8387,10 +8387,10 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G73" t="n">
         <v>80</v>
@@ -8497,10 +8497,10 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G74" t="n">
         <v>80</v>
@@ -8607,10 +8607,10 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G75" t="n">
         <v>80</v>
@@ -8717,7 +8717,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F76" t="n">
         <v>10</v>
@@ -8827,10 +8827,10 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G77" t="n">
         <v>80</v>
@@ -8937,10 +8937,10 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G78" t="n">
         <v>80</v>
@@ -9050,7 +9050,7 @@
         <v>6</v>
       </c>
       <c r="F79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G79" t="n">
         <v>80</v>
@@ -9267,10 +9267,10 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G81" t="n">
         <v>80</v>
@@ -9380,13 +9380,13 @@
         <v>7</v>
       </c>
       <c r="F82" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G82" t="n">
         <v>80</v>
       </c>
       <c r="H82" t="n">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -9487,10 +9487,10 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F83" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G83" t="n">
         <v>60</v>
@@ -9597,10 +9597,10 @@
         </is>
       </c>
       <c r="E84" t="n">
+        <v>4</v>
+      </c>
+      <c r="F84" t="n">
         <v>3</v>
-      </c>
-      <c r="F84" t="n">
-        <v>5</v>
       </c>
       <c r="G84" t="n">
         <v>60</v>
@@ -9707,10 +9707,10 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F85" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G85" t="n">
         <v>60</v>
@@ -9820,7 +9820,7 @@
         <v>7</v>
       </c>
       <c r="F86" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G86" t="n">
         <v>60</v>
@@ -9927,10 +9927,10 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G87" t="n">
         <v>80</v>
@@ -10037,10 +10037,10 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F88" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G88" t="n">
         <v>80</v>
@@ -10147,10 +10147,10 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F89" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G89" t="n">
         <v>80</v>
@@ -10257,10 +10257,10 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F90" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G90" t="n">
         <v>80</v>
@@ -10367,10 +10367,10 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F91" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G91" t="n">
         <v>80</v>
@@ -10477,10 +10477,10 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G92" t="n">
         <v>80</v>
@@ -10587,10 +10587,10 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F93" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G93" t="n">
         <v>80</v>
@@ -10697,10 +10697,10 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F94" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G94" t="n">
         <v>80</v>
@@ -10807,10 +10807,10 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F95" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G95" t="n">
         <v>80</v>
@@ -10917,10 +10917,10 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G96" t="n">
         <v>80</v>
@@ -11027,10 +11027,10 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F97" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G97" t="n">
         <v>80</v>
@@ -11137,10 +11137,10 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F98" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G98" t="n">
         <v>80</v>
@@ -11247,7 +11247,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F99" t="n">
         <v>11</v>

</xml_diff>